<commit_message>
make sure have latest f2v cal
</commit_message>
<xml_diff>
--- a/Saves/F2V_Cal20171203.xlsx
+++ b/Saves/F2V_Cal20171203.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Freq, Hz</t>
   </si>
@@ -75,24 +75,6 @@
   </si>
   <si>
     <t>dropout, vrms</t>
-  </si>
-  <si>
-    <t>ltspice</t>
-  </si>
-  <si>
-    <t>lm2917</t>
-  </si>
-  <si>
-    <t>scales</t>
-  </si>
-  <si>
-    <t>lm2907</t>
-  </si>
-  <si>
-    <t>volts</t>
-  </si>
-  <si>
-    <t>should compensate with measured voltage level</t>
   </si>
 </sst>
 </file>
@@ -202,6 +184,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1032,11 +1015,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="657421904"/>
-        <c:axId val="657422296"/>
+        <c:axId val="207832312"/>
+        <c:axId val="207835056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="657421904"/>
+        <c:axId val="207832312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,6 +1065,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1115,12 +1099,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="657422296"/>
+        <c:crossAx val="207835056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="657422296"/>
+        <c:axId val="207835056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1177,7 +1161,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="657421904"/>
+        <c:crossAx val="207832312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1191,6 +1175,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1467,11 +1452,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="657423080"/>
-        <c:axId val="657420728"/>
+        <c:axId val="202932144"/>
+        <c:axId val="202934104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="657423080"/>
+        <c:axId val="202932144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,12 +1573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="657420728"/>
+        <c:crossAx val="202934104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="657420728"/>
+        <c:axId val="202934104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1706,7 +1691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="657423080"/>
+        <c:crossAx val="202932144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2582,8 +2567,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="656349576"/>
-        <c:axId val="656351928"/>
+        <c:axId val="202932928"/>
+        <c:axId val="202934496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -2694,7 +2679,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="656349576"/>
+        <c:axId val="202932928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2812,12 +2797,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656351928"/>
+        <c:crossAx val="202934496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="656351928"/>
+        <c:axId val="202934496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2937,7 +2922,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656349576"/>
+        <c:crossAx val="202932928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5076,10 +5061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5093,7 +5078,7 @@
     <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5134,7 +5119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>150</v>
       </c>
@@ -5176,7 +5161,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>200</v>
       </c>
@@ -5216,7 +5201,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>300</v>
       </c>
@@ -5256,7 +5241,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>400</v>
       </c>
@@ -5298,7 +5283,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>450</v>
       </c>
@@ -5338,7 +5323,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>500</v>
       </c>
@@ -5378,7 +5363,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>550</v>
       </c>
@@ -5418,7 +5403,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>600</v>
       </c>
@@ -5460,7 +5445,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>650</v>
       </c>
@@ -5500,27 +5485,15 @@
         <v>39000</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="R12" t="s">
-        <v>17</v>
-      </c>
-      <c r="T12" t="s">
-        <v>18</v>
-      </c>
-      <c r="U12" t="s">
-        <v>19</v>
-      </c>
-      <c r="V12" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -5551,11 +5524,8 @@
       <c r="L13" s="2"/>
       <c r="M13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="R13" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -5586,20 +5556,8 @@
       <c r="L14" s="2"/>
       <c r="M14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="R14">
-        <v>5</v>
-      </c>
-      <c r="S14">
-        <v>650</v>
-      </c>
-      <c r="T14">
-        <v>3.19</v>
-      </c>
-      <c r="V14">
-        <v>3.1880000000000002</v>
-      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
@@ -5630,46 +5588,12 @@
       <c r="L15" s="2"/>
       <c r="M15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="R15">
-        <v>6</v>
-      </c>
-      <c r="T15">
-        <v>3.85</v>
-      </c>
-      <c r="U15">
-        <f>$T$14*R15/$R$14</f>
-        <v>3.8280000000000003</v>
-      </c>
-      <c r="V15">
-        <v>3.84</v>
-      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="R16">
-        <v>15</v>
-      </c>
-      <c r="T16">
-        <v>4.93</v>
-      </c>
-      <c r="U16">
-        <f>$T$14*R16/$R$14</f>
-        <v>9.57</v>
-      </c>
-      <c r="V16">
-        <v>9.7040000000000006</v>
-      </c>
-      <c r="W16">
-        <f>T16/T14</f>
-        <v>1.5454545454545454</v>
-      </c>
-      <c r="X16">
-        <f>R14*W16</f>
-        <v>7.7272727272727266</v>
-      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>150</v>
       </c>
@@ -5687,44 +5611,32 @@
       </c>
       <c r="M17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="R17">
-        <v>7.8</v>
-      </c>
-      <c r="T17">
-        <v>4.78</v>
-      </c>
-      <c r="V17">
-        <v>5.05</v>
-      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="U19" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24"/>

</xml_diff>